<commit_message>
Corregidor especto a base de datos final
</commit_message>
<xml_diff>
--- a/Documentación/Cocomo2.xlsx
+++ b/Documentación/Cocomo2.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\SCTps\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Primera Version (descartada)" sheetId="1" r:id="rId1"/>
+    <sheet name="Puntos de Función no Ajustados" sheetId="3" r:id="rId2"/>
+    <sheet name="Puntos de Funcion Ajustados" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="69">
   <si>
     <t>Componente</t>
   </si>
@@ -131,6 +131,108 @@
   </si>
   <si>
     <t>Puntos de función</t>
+  </si>
+  <si>
+    <t>Archivo interfaz externo</t>
+  </si>
+  <si>
+    <t>Puntos de Funcion no Ajustado</t>
+  </si>
+  <si>
+    <t>Caracteristica</t>
+  </si>
+  <si>
+    <t>Comunicación de datos</t>
+  </si>
+  <si>
+    <t>Procesamiento distribuido de datos</t>
+  </si>
+  <si>
+    <t>Rendimiento</t>
+  </si>
+  <si>
+    <t>Configuraciones fuertemente utilizadas</t>
+  </si>
+  <si>
+    <t>Frecuencia de transacciones</t>
+  </si>
+  <si>
+    <t>Entrada de datos on- line</t>
+  </si>
+  <si>
+    <t>Eficiencia del usuario final</t>
+  </si>
+  <si>
+    <t>Actualizaciones Online</t>
+  </si>
+  <si>
+    <t>Procesamiento complejo</t>
+  </si>
+  <si>
+    <t>Reusabilidad</t>
+  </si>
+  <si>
+    <t>Facilidad de instalacion</t>
+  </si>
+  <si>
+    <t>Facilidad de operación</t>
+  </si>
+  <si>
+    <t>Instalacion de distintos lugares</t>
+  </si>
+  <si>
+    <t>Facilidad de cambio</t>
+  </si>
+  <si>
+    <t>TDI</t>
+  </si>
+  <si>
+    <t>Factor de Ajuste</t>
+  </si>
+  <si>
+    <t>Puntos de Funcion</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Lineas de Codigo</t>
+  </si>
+  <si>
+    <t>Esfuerzo</t>
+  </si>
+  <si>
+    <t>Python (?</t>
+  </si>
+  <si>
+    <t>Personas</t>
+  </si>
+  <si>
+    <t>Horas por persona</t>
+  </si>
+  <si>
+    <t>Horas proyecto</t>
+  </si>
+  <si>
+    <t>Duración meses</t>
+  </si>
+  <si>
+    <t>4 horas</t>
+  </si>
+  <si>
+    <t>20 dias</t>
+  </si>
+  <si>
+    <t>80 horas x mes</t>
+  </si>
+  <si>
+    <t>5  meses y 17 dias</t>
+  </si>
+  <si>
+    <t>Puntos de Funcion no Ajustados</t>
   </si>
 </sst>
 </file>
@@ -152,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +264,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -230,12 +344,51 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -245,6 +398,234 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CuadroTexto 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="133350"/>
+          <a:ext cx="2190750" cy="1219200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>0 à No presente o sin influencia</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1 à Influencia incidental</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2 à Influencia moderada</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>3 à Influencia media</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>4 à Influencia significativa</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>5</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> à </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Fuerte influencia</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -510,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="A1:D17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,9 +1141,390 @@
         <v>23</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="1">
+        <v>3</v>
+      </c>
+      <c r="C27" s="1">
+        <v>4</v>
+      </c>
+      <c r="D27" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="1">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D53" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53" s="7">
+        <f>SUM(E37:E52)</f>
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B36:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -771,112 +1533,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A2:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="5" width="19.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="1">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="1">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="1">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:M7"/>
+    <sheetView zoomScale="35" zoomScaleNormal="35" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,269 +1546,504 @@
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="3">
+        <f>'Puntos de Función no Ajustados'!C288</f>
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="H10" s="1">
+        <f>(B10*C10)+(D10*E10)+(F10*G10)</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>7</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" ref="H11:H14" si="0">(B11*C11)+(D11*E11)+(F11*G11)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="G13" s="1">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="1"/>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="9">
+        <f>SUM(H10:H14)</f>
+        <v>213</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="1">
+        <f>SUM(F2:F15)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="1">
+        <f>(F16*0.01)+0.65</f>
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1">
+        <f>1.06*213</f>
+        <v>225.78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="1">
+        <f>B20*60</f>
+        <v>13546.8</v>
+      </c>
+      <c r="C21">
+        <v>65</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="1">
+        <f>B20/(1/8)</f>
+        <v>1806.24</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1806.24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="1">
+        <f>B23/C22</f>
+        <v>451.56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="9">
+        <f>B24/80</f>
+        <v>5.6444999999999999</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>